<commit_message>
Update to the descriptives
</commit_message>
<xml_diff>
--- a/Data/Raw data/modena_final_2008_2018.xlsx
+++ b/Data/Raw data/modena_final_2008_2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tl0\Documents\R\modena_carbapenem_resistance\Data\Raw data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C610ADC-43C2-459F-8126-724314289912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B2FD10-AECC-4E8D-8A69-B5C5FDF34FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1627,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IM133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="AQ28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="BU60" sqref="BU60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -44944,6 +44944,9 @@
       <c r="BT59">
         <v>6</v>
       </c>
+      <c r="BU59">
+        <v>16</v>
+      </c>
       <c r="BV59">
         <v>0</v>
       </c>

</xml_diff>